<commit_message>
functionality for detecting tables working sometimes
</commit_message>
<xml_diff>
--- a/out/CBP/Øko_konventionelt Nordsjælands hospitaler juli.xlsx
+++ b/out/CBP/Øko_konventionelt Nordsjælands hospitaler juli.xlsx
@@ -8,21 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Øko_konventionelt køb i kg Nord" sheetId="1" r:id="rId6"/>
+    <sheet name="FirstPass" sheetId="2" r:id="rId7"/>
+    <sheet name="SecondPass" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="1" fullPrecision="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">Sygehus lillebælt   Periode 01-07-2024 - 31-07-2024</t>
-  </si>
-  <si>
-    <t>4% filler,47% containsProductNr,47% containsAmount,</t>
-  </si>
-  <si>
-    <t>9% filler,90% NrHeader,</t>
   </si>
   <si>
     <t xml:space="preserve">Faktura Nr </t>
@@ -57,63 +53,69 @@
     <t xml:space="preserve">Mængde kg </t>
   </si>
   <si>
+    <t>620308</t>
+  </si>
+  <si>
+    <t>20130</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>20130 ~ Øko Mørk Brødmalt 12,5 kg</t>
+  </si>
+  <si>
+    <t>620308 ~ Nordsjællands Hospital</t>
+  </si>
+  <si>
+    <t>36018</t>
+  </si>
+  <si>
+    <t>Nej</t>
+  </si>
+  <si>
+    <t>36018 ~ Kronjäst orig. gær 12x1 kg</t>
+  </si>
+  <si>
+    <t>82685</t>
+  </si>
+  <si>
+    <t>82685 ~ 1/2 Palle</t>
+  </si>
+  <si>
+    <t>944696</t>
+  </si>
+  <si>
+    <t>944696 ~ Credifrost® Super 12,5 kg</t>
+  </si>
+  <si>
+    <t>99100</t>
+  </si>
+  <si>
+    <t>99100 ~ Energitillæg</t>
+  </si>
+  <si>
+    <t>4% filler,47% containsProductNr,47% containsAmount,</t>
+  </si>
+  <si>
+    <t>9% filler,90% NrHeader,</t>
+  </si>
+  <si>
     <t>4% filler,47% productNameHeader,47% NrHeader,</t>
   </si>
   <si>
-    <t>620308</t>
-  </si>
-  <si>
-    <t>20130</t>
-  </si>
-  <si>
-    <t>Ja</t>
-  </si>
-  <si>
-    <t>20130 ~ Øko Mørk Brødmalt 12,5 kg</t>
-  </si>
-  <si>
-    <t>620308 ~ Nordsjællands Hospital</t>
-  </si>
-  <si>
     <t>9% filler,90% QuantityHeader,</t>
   </si>
   <si>
-    <t>36018</t>
-  </si>
-  <si>
-    <t>Nej</t>
-  </si>
-  <si>
-    <t>36018 ~ Kronjäst orig. gær 12x1 kg</t>
-  </si>
-  <si>
     <t>3% filler,32% SingleMassHeader,32% TotalMassHeader,32% QuantityHeader,</t>
   </si>
   <si>
-    <t>82685</t>
-  </si>
-  <si>
-    <t>82685 ~ 1/2 Palle</t>
-  </si>
-  <si>
     <t>5% filler,10% containsTotalMass,10% containsSingleMass,52% isInteger,10% containsProductNr,10% containsAmount,</t>
   </si>
   <si>
-    <t>944696</t>
-  </si>
-  <si>
-    <t>944696 ~ Credifrost® Super 12,5 kg</t>
-  </si>
-  <si>
     <t>1% filler,15% containsTotalMass,15% containsSingleMass,15% containsProduct,7% containsProductNr,15% containsAmount,15% SingleMassHeader,15% TotalMassHeader,</t>
   </si>
   <si>
-    <t>99100</t>
-  </si>
-  <si>
-    <t>99100 ~ Energitillæg</t>
-  </si>
-  <si>
     <t>6% filler,31% containsProductNr,62% containsAmount,</t>
   </si>
   <si>
@@ -121,6 +123,24 @@
   </si>
   <si>
     <t>4% filler,23% containsTotalMass,23% containsSingleMass,47% isDecimal,</t>
+  </si>
+  <si>
+    <t>2% filler,21% containsSingleMass,21% containsProduct,10% containsProductNr,21% containsAmount,21% SingleMassHeader,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARENR, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARENR, ANTAL, STK. MASSE, TOTAL MASSE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRODUKT, VARENR, ANTAL, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARENR, ANTAL, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANTAL, STK. MASSE, TOTAL MASSE </t>
   </si>
 </sst>
 </file>
@@ -156,7 +176,7 @@
       <name val="Segoe UI"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,6 +291,46 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE3DD42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF747D9B"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF747D9B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF006400"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2E8B57"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -315,16 +375,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="82" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
@@ -371,6 +443,34 @@
     <xf numFmtId="0" fontId="0" fillId="21" applyFill="1" borderId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="16" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="22" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" applyFill="1" borderId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="24" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="25" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="26" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="82" applyNumberFormat="1" fontId="4" applyFont="1" fillId="27" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="28" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="27" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="27" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="82" applyNumberFormat="1" fontId="4" applyFont="1" fillId="28" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,7 +554,7 @@
   <sheetPr>
     <outlinePr/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0"/>
   </sheetViews>
@@ -474,226 +574,685 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="5" t="s">
+    </row>
+    <row r="2" ht="4" customHeight="1"/>
+    <row r="3" ht="19.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" ht="19.25">
+      <c r="A4" s="4">
+        <v>1228259</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="4">
+        <v>625</v>
+      </c>
+      <c r="J4" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" ht="19.25">
+      <c r="A5" s="4">
+        <v>1228259</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="4">
+        <v>205.2</v>
+      </c>
+      <c r="J5" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" ht="19.3">
+      <c r="A6" s="4">
+        <v>1228259</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="4">
+        <v>55</v>
+      </c>
+      <c r="J6" s="4">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="7" ht="19.25">
+      <c r="A7" s="4">
+        <v>1228259</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2355</v>
+      </c>
+      <c r="J7" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" ht="19.2">
+      <c r="A8" s="4">
+        <v>1228259</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="4">
+        <v>111</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" ht="0.05" customHeight="1"/>
+    <row r="10" ht="20.45" customHeight="1"/>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.78740157480315" right="0.78740157480315" top="0.78740157480315" bottom="1.23740157480315" header="0.78740157480315" footer="0.78740157480315"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddFooter>&amp;C&amp;"Segoe UI,Regular"&amp;10 8/1/2024 7:45:04 AM </oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="13.4921875" customWidth="1"/>
+    <col min="2" max="2" width="13.50390625" customWidth="1"/>
+    <col min="3" max="3" width="13.4921875" customWidth="1"/>
+    <col min="4" max="4" width="10.78125" customWidth="1"/>
+    <col min="5" max="5" width="24.15234375" customWidth="1"/>
+    <col min="6" max="6" width="20.421875" customWidth="1"/>
+    <col min="7" max="7" width="13.4921875" customWidth="1"/>
+    <col min="8" max="8" width="35.0625" customWidth="1"/>
+    <col min="9" max="9" width="18.640625" customWidth="1"/>
+    <col min="10" max="10" width="15.9140625" customWidth="1"/>
+    <col min="11" max="11" width="0.0234375" customWidth="1"/>
+    <col min="12" max="12" width="26.9921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="28.5" customHeight="1">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2" ht="4" customHeight="1">
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" ht="19.25">
+      <c r="A3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
-    </row>
+      <c r="C3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" ht="19.25">
+      <c r="A4" s="18">
+        <v>1228259</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="18">
+        <v>625</v>
+      </c>
+      <c r="J4" s="18">
+        <v>25</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" ht="19.25">
+      <c r="A5" s="18">
+        <v>1228259</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="27">
+        <v>205.2</v>
+      </c>
+      <c r="J5" s="18">
+        <v>12</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" ht="19.3">
+      <c r="A6" s="18">
+        <v>1228259</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="18">
+        <v>55</v>
+      </c>
+      <c r="J6" s="27">
+        <v>10.6</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" ht="19.25">
+      <c r="A7" s="18">
+        <v>1228259</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="18">
+        <v>2355</v>
+      </c>
+      <c r="J7" s="18">
+        <v>50</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" ht="19.2">
+      <c r="A8" s="18">
+        <v>1228259</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="18">
+        <v>111</v>
+      </c>
+      <c r="J8" s="18">
+        <v>0</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" ht="0.05" customHeight="1">
+      <c r="K9" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" ht="20.45" customHeight="1">
+      <c r="K10" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="K11" s="31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.78740157480315" right="0.78740157480315" top="0.78740157480315" bottom="1.23740157480315" header="0.78740157480315" footer="0.78740157480315"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddFooter>&amp;C&amp;"Segoe UI,Regular"&amp;10 8/1/2024 7:45:04 AM </oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="13.4921875" customWidth="1"/>
+    <col min="2" max="2" width="13.50390625" customWidth="1"/>
+    <col min="3" max="3" width="13.4921875" customWidth="1"/>
+    <col min="4" max="4" width="10.78125" customWidth="1"/>
+    <col min="5" max="5" width="24.15234375" customWidth="1"/>
+    <col min="6" max="6" width="20.421875" customWidth="1"/>
+    <col min="7" max="7" width="13.4921875" customWidth="1"/>
+    <col min="8" max="8" width="35.0625" customWidth="1"/>
+    <col min="9" max="9" width="18.640625" customWidth="1"/>
+    <col min="10" max="10" width="15.9140625" customWidth="1"/>
+    <col min="11" max="11" width="0.0234375" customWidth="1"/>
+    <col min="12" max="12" width="26.9921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="28.5" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" ht="4" customHeight="1"/>
     <row r="3" ht="19.25">
-      <c r="A3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="33"/>
+      <c r="G3" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" ht="19.25">
+      <c r="A4" s="35">
+        <v>1228259</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" ht="19.25">
-      <c r="A4" s="14">
-        <v>1228259</v>
-      </c>
-      <c r="B4" s="16" t="s">
+      <c r="E4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="4">
+        <v>625</v>
+      </c>
+      <c r="J4" s="39">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" ht="19.25">
+      <c r="A5" s="35">
+        <v>1228259</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="D5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="19" t="s">
+      <c r="E5" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="14">
-        <v>625</v>
-      </c>
-      <c r="J4" s="14">
-        <v>25</v>
-      </c>
-      <c r="K4" s="11" t="s">
+      <c r="F5" s="3"/>
+      <c r="G5" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="4">
+        <v>205.2</v>
+      </c>
+      <c r="J5" s="39">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" ht="19.3">
+      <c r="A6" s="4">
+        <v>1228259</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" ht="19.25">
-      <c r="A5" s="14">
-        <v>1228259</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="16" t="s">
+      <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="F6" s="3"/>
+      <c r="G6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="4">
+        <v>55</v>
+      </c>
+      <c r="J6" s="4">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="7" ht="19.25">
+      <c r="A7" s="4">
+        <v>1228259</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="D7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="23">
-        <v>205.2</v>
-      </c>
-      <c r="J5" s="14">
-        <v>12</v>
-      </c>
-      <c r="K5" s="13" t="s">
+      <c r="F7" s="3"/>
+      <c r="G7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2355</v>
+      </c>
+      <c r="J7" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" ht="19.2">
+      <c r="A8" s="4">
+        <v>1228259</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" ht="19.3">
-      <c r="A6" s="14">
-        <v>1228259</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="16" t="s">
+      <c r="D8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="14">
-        <v>55</v>
-      </c>
-      <c r="J6" s="23">
-        <v>10.6</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" ht="19.25">
-      <c r="A7" s="14">
-        <v>1228259</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="14">
-        <v>2355</v>
-      </c>
-      <c r="J7" s="14">
-        <v>50</v>
-      </c>
-      <c r="K7" s="18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" ht="19.2">
-      <c r="A8" s="14">
-        <v>1228259</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="14">
+      <c r="F8" s="3"/>
+      <c r="G8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="4">
         <v>111</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="4">
         <v>0</v>
       </c>
-      <c r="K8" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" ht="0.05" customHeight="1">
-      <c r="K9" s="22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" ht="20.45" customHeight="1">
-      <c r="K10" s="24" t="s">
-        <v>32</v>
-      </c>
-    </row>
+    </row>
+    <row r="9" ht="0.05" customHeight="1"/>
+    <row r="10" ht="20.45" customHeight="1"/>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:E1"/>

</xml_diff>